<commit_message>
test spec revision - cipher change to DES-CBC3-MD5
</commit_message>
<xml_diff>
--- a/docs/testspec/RICO_13351_TestSpec03.xlsx
+++ b/docs/testspec/RICO_13351_TestSpec03.xlsx
@@ -190,9 +190,6 @@
     <t>DES-CBC-MD5</t>
   </si>
   <si>
-    <t>RC2-CBC-MD5</t>
-  </si>
-  <si>
     <t>TSCN02(A/B)</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>TLSv1,SSLv3,SSLv2</t>
+  </si>
+  <si>
+    <t>DES-CBC3-MD5</t>
   </si>
   <si>
     <t>Nmap script shows result as 'TLS_FALLBACK_SCSV properly implemented'</t>
@@ -457,6 +457,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -481,9 +499,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -495,21 +510,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1471,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1492,26 +1492,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="20.25">
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="2:9" ht="14.25" customHeight="1">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="2:9" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="C3" s="4"/>
@@ -1539,11 +1539,11 @@
       <c r="C5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1837,10 +1837,10 @@
         <v>4</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>48</v>
@@ -1864,7 +1864,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>7</v>
@@ -1891,7 +1891,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>7</v>
@@ -1918,7 +1918,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>5</v>
@@ -1945,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>5</v>
@@ -1966,7 +1966,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>4</v>
@@ -1993,7 +1993,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>4</v>
@@ -2020,7 +2020,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>4</v>
@@ -2047,7 +2047,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>4</v>
@@ -2074,7 +2074,7 @@
         <v>10</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>4</v>
@@ -2107,7 +2107,7 @@
         <v>13</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>7</v>
@@ -2134,7 +2134,7 @@
         <v>13</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>5</v>
@@ -2161,7 +2161,7 @@
         <v>13</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>5</v>
@@ -2367,222 +2367,222 @@
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29" t="s">
+      <c r="D58" s="17"/>
+      <c r="E58" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="29"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
     </row>
     <row r="60" spans="2:10">
       <c r="B60" s="10">
         <v>1</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C60" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D60" s="15"/>
-      <c r="E60" s="22" t="s">
+      <c r="D60" s="21"/>
+      <c r="E60" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F60" s="27"/>
-      <c r="G60" s="27"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
     </row>
     <row r="61" spans="2:10">
       <c r="B61" s="10">
         <v>2</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="22" t="s">
+      <c r="C61" s="22"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
     </row>
     <row r="62" spans="2:10">
       <c r="B62" s="10">
         <v>3</v>
       </c>
-      <c r="C62" s="16"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="22" t="s">
+      <c r="C62" s="22"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
     </row>
     <row r="63" spans="2:10">
       <c r="B63" s="10">
         <v>4</v>
       </c>
-      <c r="C63" s="16"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="22" t="s">
+      <c r="C63" s="22"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="27"/>
-      <c r="G63" s="27"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" s="10">
         <v>5</v>
       </c>
-      <c r="C64" s="16"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="22" t="s">
+      <c r="C64" s="22"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
     </row>
     <row r="65" spans="2:7">
       <c r="B65" s="10">
         <v>6</v>
       </c>
-      <c r="C65" s="16"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="22" t="s">
+      <c r="C65" s="22"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
     </row>
     <row r="66" spans="2:7">
       <c r="B66" s="10">
         <v>7</v>
       </c>
-      <c r="C66" s="16"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="22" t="s">
+      <c r="C66" s="22"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F66" s="27"/>
-      <c r="G66" s="27"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
     </row>
     <row r="67" spans="2:7">
       <c r="B67" s="10">
         <v>8</v>
       </c>
-      <c r="C67" s="16"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="22" t="s">
+      <c r="C67" s="22"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
     </row>
     <row r="68" spans="2:7">
       <c r="B68" s="10">
         <v>9</v>
       </c>
-      <c r="C68" s="16"/>
-      <c r="D68" s="17"/>
-      <c r="E68" s="22" t="s">
+      <c r="C68" s="22"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
     </row>
     <row r="69" spans="2:7">
       <c r="B69" s="10">
         <v>10</v>
       </c>
-      <c r="C69" s="16"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="22" t="s">
+      <c r="C69" s="22"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
     </row>
     <row r="70" spans="2:7">
       <c r="B70" s="10">
         <v>11</v>
       </c>
-      <c r="C70" s="16"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="22" t="s">
+      <c r="C70" s="22"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F70" s="27"/>
-      <c r="G70" s="27"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
     </row>
     <row r="71" spans="2:7">
       <c r="B71" s="10">
         <v>12</v>
       </c>
-      <c r="C71" s="16"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="22" t="s">
+      <c r="C71" s="22"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F71" s="27"/>
-      <c r="G71" s="27"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
     </row>
     <row r="72" spans="2:7">
       <c r="B72" s="10">
         <v>13</v>
       </c>
-      <c r="C72" s="16"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="20" t="s">
+      <c r="C72" s="22"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F72" s="21"/>
-      <c r="G72" s="22"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="14"/>
     </row>
     <row r="73" spans="2:7">
       <c r="B73" s="10">
         <v>14</v>
       </c>
-      <c r="C73" s="18"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="20" t="s">
+      <c r="C73" s="24"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="F73" s="21"/>
-      <c r="G73" s="22"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="14"/>
     </row>
     <row r="74" spans="2:7">
       <c r="B74" s="10">
         <v>15</v>
       </c>
-      <c r="C74" s="23" t="s">
+      <c r="C74" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D74" s="24"/>
-      <c r="E74" s="20" t="s">
+      <c r="D74" s="29"/>
+      <c r="E74" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F74" s="21"/>
-      <c r="G74" s="22"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="14"/>
     </row>
     <row r="75" spans="2:7">
       <c r="B75" s="10">
         <v>16</v>
       </c>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-      <c r="E75" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F75" s="21"/>
-      <c r="G75" s="22"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F75" s="27"/>
+      <c r="G75" s="14"/>
     </row>
     <row r="76" spans="2:7">
       <c r="E76" s="3"/>
@@ -2598,6 +2598,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="C74:D75"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
     <mergeCell ref="E71:G71"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="B58:B59"/>
@@ -2609,19 +2619,9 @@
     <mergeCell ref="C60:D73"/>
     <mergeCell ref="E72:G72"/>
     <mergeCell ref="E73:G73"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="C74:D75"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
     <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E68:G68"/>
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
5103 Test results, evidence, installation batch file and source zip added
</commit_message>
<xml_diff>
--- a/docs/testspec/RICO_13351_TestSpec03.xlsx
+++ b/docs/testspec/RICO_13351_TestSpec03.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="62">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>AES128-SHA</t>
-  </si>
-  <si>
-    <t>IDEA-CBC-SHA</t>
   </si>
   <si>
     <t>EDH-RSA-DES-CBC-SHA</t>
@@ -208,7 +205,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$₹-4009]#,##0.00;[Red]&quot;-&quot;[$₹-4009]#,##0.00"/>
   </numFmts>
@@ -457,9 +454,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -492,27 +510,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1257,7 +1254,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1292,7 +1288,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1468,11 +1463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J79"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1492,26 +1487,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="20.25">
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="2:9" ht="14.25" customHeight="1">
+      <c r="C2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="2:9" ht="14.25" customHeight="1">
-      <c r="C2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="2:9" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="C3" s="4"/>
@@ -1526,7 +1521,7 @@
     </row>
     <row r="4" spans="2:9" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1537,13 +1532,13 @@
     </row>
     <row r="5" spans="2:9" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -1598,7 +1593,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1615,10 +1610,10 @@
     </row>
     <row r="13" spans="2:9" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
@@ -1667,7 +1662,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1675,10 +1670,10 @@
     </row>
     <row r="19" spans="2:10" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="C19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3"/>
@@ -1724,14 +1719,14 @@
     </row>
     <row r="24" spans="2:10" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="C24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1777,7 +1772,7 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1794,7 +1789,7 @@
     </row>
     <row r="31" spans="2:10" ht="18">
       <c r="B31" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="2:10" s="9" customFormat="1" ht="38.25">
@@ -1805,16 +1800,16 @@
         <v>0</v>
       </c>
       <c r="D32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="G32" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>2</v>
@@ -1823,7 +1818,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="25.5">
@@ -1831,25 +1826,25 @@
         <v>1</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I33" s="32" t="s">
-        <v>62</v>
+      <c r="I33" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="J33" s="10"/>
     </row>
@@ -1858,19 +1853,19 @@
         <v>2</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>6</v>
@@ -1885,19 +1880,19 @@
         <v>3</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>9</v>
@@ -1912,19 +1907,19 @@
         <v>4</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>6</v>
@@ -1939,19 +1934,19 @@
         <v>5</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>9</v>
@@ -1966,7 +1961,7 @@
         <v>6</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>4</v>
@@ -1978,7 +1973,7 @@
         <v>7</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>11</v>
@@ -1993,7 +1988,7 @@
         <v>7</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>4</v>
@@ -2005,7 +2000,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H39" s="10" t="s">
         <v>11</v>
@@ -2020,7 +2015,7 @@
         <v>8</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>4</v>
@@ -2032,7 +2027,7 @@
         <v>7</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H40" s="10" t="s">
         <v>11</v>
@@ -2047,7 +2042,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>4</v>
@@ -2059,7 +2054,7 @@
         <v>5</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>11</v>
@@ -2074,19 +2069,19 @@
         <v>10</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>11</v>
@@ -2101,19 +2096,19 @@
         <v>11</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>11</v>
@@ -2128,19 +2123,19 @@
         <v>12</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" s="10" t="s">
         <v>6</v>
@@ -2155,19 +2150,19 @@
         <v>13</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F45" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>9</v>
@@ -2182,7 +2177,7 @@
         <v>14</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>13</v>
@@ -2194,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H46" s="10" t="s">
         <v>11</v>
@@ -2209,7 +2204,7 @@
         <v>15</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>13</v>
@@ -2221,7 +2216,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H47" s="10" t="s">
         <v>11</v>
@@ -2236,7 +2231,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>13</v>
@@ -2248,7 +2243,7 @@
         <v>7</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>11</v>
@@ -2263,7 +2258,7 @@
         <v>17</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>13</v>
@@ -2275,7 +2270,7 @@
         <v>5</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H49" s="10" t="s">
         <v>11</v>
@@ -2290,19 +2285,19 @@
         <v>18</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H50" s="10" t="s">
         <v>11</v>
@@ -2358,7 +2353,7 @@
     </row>
     <row r="57" spans="2:10" ht="18">
       <c r="B57" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2367,225 +2362,216 @@
       <c r="H57" s="2"/>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17" t="s">
+      <c r="B58" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="17"/>
-      <c r="G58" s="17"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
     </row>
     <row r="60" spans="2:10">
       <c r="B60" s="10">
         <v>1</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="21"/>
-      <c r="E60" s="14" t="s">
+      <c r="C60" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="28"/>
+      <c r="E60" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
     </row>
     <row r="61" spans="2:10">
       <c r="B61" s="10">
         <v>2</v>
       </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="14" t="s">
+      <c r="C61" s="29"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
     </row>
     <row r="62" spans="2:10">
       <c r="B62" s="10">
         <v>3</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="23"/>
-      <c r="E62" s="14" t="s">
+      <c r="C62" s="29"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
+      <c r="F62" s="22"/>
+      <c r="G62" s="22"/>
     </row>
     <row r="63" spans="2:10">
       <c r="B63" s="10">
         <v>4</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="14" t="s">
+      <c r="C63" s="29"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
     </row>
     <row r="64" spans="2:10">
       <c r="B64" s="10">
         <v>5</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="14" t="s">
+      <c r="C64" s="29"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
+      <c r="F64" s="22"/>
+      <c r="G64" s="22"/>
     </row>
     <row r="65" spans="2:7">
       <c r="B65" s="10">
         <v>6</v>
       </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="14" t="s">
+      <c r="C65" s="29"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
     </row>
     <row r="66" spans="2:7">
       <c r="B66" s="10">
         <v>7</v>
       </c>
-      <c r="C66" s="22"/>
-      <c r="D66" s="23"/>
-      <c r="E66" s="14" t="s">
+      <c r="C66" s="29"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
     </row>
     <row r="67" spans="2:7">
       <c r="B67" s="10">
         <v>8</v>
       </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="14" t="s">
+      <c r="C67" s="29"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="22"/>
     </row>
     <row r="68" spans="2:7">
       <c r="B68" s="10">
         <v>9</v>
       </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="14" t="s">
+      <c r="C68" s="29"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
+      <c r="F68" s="22"/>
+      <c r="G68" s="22"/>
     </row>
     <row r="69" spans="2:7">
       <c r="B69" s="10">
         <v>10</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="14" t="s">
+      <c r="C69" s="29"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
     </row>
     <row r="70" spans="2:7">
       <c r="B70" s="10">
         <v>11</v>
       </c>
-      <c r="C70" s="22"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="14" t="s">
+      <c r="C70" s="29"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
     </row>
     <row r="71" spans="2:7">
       <c r="B71" s="10">
         <v>12</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" s="15"/>
-      <c r="G71" s="15"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F71" s="16"/>
+      <c r="G71" s="17"/>
     </row>
     <row r="72" spans="2:7">
       <c r="B72" s="10">
         <v>13</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="26" t="s">
+      <c r="C72" s="31"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="F72" s="27"/>
-      <c r="G72" s="14"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="17"/>
     </row>
     <row r="73" spans="2:7">
       <c r="B73" s="10">
         <v>14</v>
       </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="26" t="s">
+      <c r="C73" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F73" s="27"/>
-      <c r="G73" s="14"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F73" s="16"/>
+      <c r="G73" s="17"/>
     </row>
     <row r="74" spans="2:7">
       <c r="B74" s="10">
         <v>15</v>
       </c>
-      <c r="C74" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D74" s="29"/>
-      <c r="E74" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F74" s="27"/>
-      <c r="G74" s="14"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F74" s="16"/>
+      <c r="G74" s="17"/>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="10">
-        <v>16</v>
-      </c>
-      <c r="C75" s="30"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F75" s="27"/>
-      <c r="G75" s="14"/>
+      <c r="E75" s="3"/>
     </row>
     <row r="76" spans="2:7">
-      <c r="E76" s="3"/>
+      <c r="E76" s="2"/>
     </row>
     <row r="77" spans="2:7">
       <c r="E77" s="2"/>
@@ -2593,22 +2579,8 @@
     <row r="78" spans="2:7">
       <c r="E78" s="2"/>
     </row>
-    <row r="79" spans="2:7">
-      <c r="E79" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="C74:D75"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
+  <mergeCells count="23">
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="C1:I1"/>
@@ -2616,12 +2588,22 @@
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="C58:D59"/>
     <mergeCell ref="E58:G59"/>
-    <mergeCell ref="C60:D73"/>
+    <mergeCell ref="C60:D72"/>
+    <mergeCell ref="E71:G71"/>
     <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E73:G73"/>
     <mergeCell ref="E61:G61"/>
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="C73:D74"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>